<commit_message>
Update : Complete MAS Report processor
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx-templates/mas-report-6a.xlsx
+++ b/src/main/resources/xlsx-templates/mas-report-6a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProject\dtc-portal-api\src\main\resources\xlsx-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProject\dtc-settlement-engine\src\main\resources\xlsx-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF347233-856A-4DF5-B551-C1DF78F4553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9E3208-5993-47C3-AF05-9776597937A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -370,9 +370,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -415,16 +415,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -710,12 +710,8 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="9">
-        <v>20</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>

</xml_diff>

<commit_message>
Update : Adjust MAS Report format and data
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx-templates/mas-report-6a.xlsx
+++ b/src/main/resources/xlsx-templates/mas-report-6a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProject\dtc-settlement-engine\src\main\resources\xlsx-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F0C56-80F9-4B98-9239-8359B2EAED7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091AA87-AF9F-4AE6-94F4-A08E4C5D5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,8 +397,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -424,11 +424,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +648,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -700,20 +700,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="10"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>